<commit_message>
Commit for big review A
</commit_message>
<xml_diff>
--- a/MCUPinAllocations.xlsx
+++ b/MCUPinAllocations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\n9733833\Documents\QUTMS_Radio\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2E923878-5983-46AE-9AEE-4E0E40B9884F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27272297-18B1-4033-8DB6-FD82B0353E08}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" activeTab="1" xr2:uid="{C87B3ED6-484C-4CA1-8124-53CAC5FECB2E}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{C87B3ED6-484C-4CA1-8124-53CAC5FECB2E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -555,26 +555,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -592,6 +577,21 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -909,18 +909,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E7DCE52-D4A2-4ADB-9EF7-0365738163B8}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="A1:I145"/>
   <sheetViews>
-    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="H48" sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A85" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="H44" sqref="H44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="1"/>
-    <col min="3" max="3" width="8.42578125" style="6" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.42578125" style="7" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="2.140625" style="7" customWidth="1"/>
+    <col min="3" max="3" width="8.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="2.140625" style="3" customWidth="1"/>
     <col min="6" max="6" width="18.7109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="2.140625" customWidth="1"/>
     <col min="8" max="8" width="29.85546875" bestFit="1" customWidth="1"/>
@@ -934,62 +937,62 @@
       <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="D1" s="9"/>
-      <c r="E1" s="8"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="4"/>
       <c r="F1" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="11" t="s">
         <v>2</v>
       </c>
       <c r="B2">
         <v>1</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="7">
+      <c r="D2" s="3">
         <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="2"/>
+      <c r="A3" s="11"/>
       <c r="B3">
         <v>2</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="7">
+      <c r="D3" s="3">
         <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="2"/>
+      <c r="A4" s="11"/>
       <c r="B4">
         <v>3</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="C4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="7">
+      <c r="D4" s="3">
         <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="2"/>
+      <c r="A5" s="11"/>
       <c r="B5">
         <v>4</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="C5" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="7">
+      <c r="D5" s="3">
         <v>5</v>
       </c>
       <c r="H5" t="s">
@@ -997,120 +1000,120 @@
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="2"/>
+      <c r="A6" s="11"/>
       <c r="B6">
         <v>5</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="C6" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D6" s="7">
+      <c r="D6" s="3">
         <v>6</v>
       </c>
       <c r="H6" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="7" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="2"/>
-      <c r="B7" s="13">
+    <row r="7" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="11"/>
+      <c r="B7" s="8">
         <v>6</v>
       </c>
-      <c r="C7" s="14" t="s">
+      <c r="C7" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="D7" s="15"/>
-      <c r="E7" s="15"/>
+      <c r="D7" s="10"/>
+      <c r="E7" s="10"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="2"/>
+      <c r="A8" s="11"/>
       <c r="B8">
         <v>7</v>
       </c>
-      <c r="C8" s="6" t="s">
+      <c r="C8" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D8" s="7">
+      <c r="D8" s="3">
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="2"/>
-      <c r="B9" s="10">
+    <row r="9" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="11"/>
+      <c r="B9" s="5">
         <v>8</v>
       </c>
-      <c r="C9" s="11" t="s">
+      <c r="C9" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="D9" s="12">
+      <c r="D9" s="7">
         <v>14</v>
       </c>
-      <c r="E9" s="12"/>
-      <c r="F9" s="10" t="s">
+      <c r="E9" s="7"/>
+      <c r="F9" s="5" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="10" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="2"/>
-      <c r="B10" s="10">
-        <v>9</v>
-      </c>
-      <c r="C10" s="11" t="s">
+    <row r="10" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="11"/>
+      <c r="B10" s="5">
+        <v>9</v>
+      </c>
+      <c r="C10" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="D10" s="12">
+      <c r="D10" s="7">
         <v>15</v>
       </c>
-      <c r="E10" s="12"/>
-      <c r="F10" s="10" t="s">
+      <c r="E10" s="7"/>
+      <c r="F10" s="5" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="2"/>
+      <c r="A11" s="11"/>
       <c r="B11">
         <v>10</v>
       </c>
-      <c r="C11" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="D11" s="7">
+      <c r="C11" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D11" s="3">
         <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="2"/>
+      <c r="A12" s="11"/>
       <c r="B12">
         <v>11</v>
       </c>
-      <c r="C12" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="D12" s="7">
+      <c r="C12" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D12" s="3">
         <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="2"/>
+      <c r="A13" s="11"/>
       <c r="B13">
         <v>12</v>
       </c>
-      <c r="C13" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="D13" s="7">
+      <c r="C13" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D13" s="3">
         <v>2</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="2"/>
+      <c r="A14" s="11"/>
       <c r="B14">
         <v>13</v>
       </c>
-      <c r="C14" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="D14" s="7">
+      <c r="C14" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D14" s="3">
         <v>3</v>
       </c>
       <c r="I14" t="s">
@@ -1118,14 +1121,14 @@
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="2"/>
+      <c r="A15" s="11"/>
       <c r="B15">
         <v>14</v>
       </c>
-      <c r="C15" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="D15" s="7">
+      <c r="C15" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D15" s="3">
         <v>4</v>
       </c>
       <c r="I15" t="s">
@@ -1133,51 +1136,51 @@
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="2"/>
+      <c r="A16" s="11"/>
       <c r="B16">
         <v>15</v>
       </c>
-      <c r="C16" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="D16" s="7">
+      <c r="C16" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D16" s="3">
         <v>5</v>
       </c>
       <c r="I16" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="17" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="2"/>
-      <c r="B17" s="13">
+    <row r="17" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="11"/>
+      <c r="B17" s="8">
         <v>16</v>
       </c>
-      <c r="C17" s="14" t="s">
+      <c r="C17" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="D17" s="15"/>
-      <c r="E17" s="15"/>
-    </row>
-    <row r="18" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="2"/>
-      <c r="B18" s="13">
+      <c r="D17" s="10"/>
+      <c r="E17" s="10"/>
+    </row>
+    <row r="18" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="11"/>
+      <c r="B18" s="8">
         <v>17</v>
       </c>
-      <c r="C18" s="14" t="s">
+      <c r="C18" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="D18" s="15"/>
-      <c r="E18" s="15"/>
+      <c r="D18" s="10"/>
+      <c r="E18" s="10"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A19" s="2"/>
+      <c r="A19" s="11"/>
       <c r="B19">
         <v>18</v>
       </c>
-      <c r="C19" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="D19" s="7">
+      <c r="C19" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D19" s="3">
         <v>6</v>
       </c>
       <c r="H19" t="s">
@@ -1188,14 +1191,14 @@
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A20" s="2"/>
+      <c r="A20" s="11"/>
       <c r="B20">
         <v>19</v>
       </c>
-      <c r="C20" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="D20" s="7">
+      <c r="C20" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D20" s="3">
         <v>7</v>
       </c>
       <c r="H20" t="s">
@@ -1206,14 +1209,14 @@
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A21" s="2"/>
+      <c r="A21" s="11"/>
       <c r="B21">
         <v>20</v>
       </c>
-      <c r="C21" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="D21" s="7">
+      <c r="C21" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D21" s="3">
         <v>7</v>
       </c>
       <c r="H21" t="s">
@@ -1224,14 +1227,14 @@
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A22" s="2"/>
+      <c r="A22" s="11"/>
       <c r="B22">
         <v>21</v>
       </c>
-      <c r="C22" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="D22" s="7">
+      <c r="C22" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D22" s="3">
         <v>9</v>
       </c>
       <c r="H22" t="s">
@@ -1242,14 +1245,14 @@
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A23" s="2"/>
+      <c r="A23" s="11"/>
       <c r="B23">
         <v>22</v>
       </c>
-      <c r="C23" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="D23" s="7">
+      <c r="C23" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D23" s="3">
         <v>10</v>
       </c>
       <c r="H23" t="s">
@@ -1259,58 +1262,58 @@
         <v>86</v>
       </c>
     </row>
-    <row r="24" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="2"/>
-      <c r="B24" s="10">
+    <row r="24" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="11"/>
+      <c r="B24" s="5">
         <v>23</v>
       </c>
-      <c r="C24" s="11" t="s">
+      <c r="C24" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="D24" s="12">
+      <c r="D24" s="7">
         <v>0</v>
       </c>
-      <c r="E24" s="12"/>
-      <c r="F24" s="10" t="s">
+      <c r="E24" s="7"/>
+      <c r="F24" s="5" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="25" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="2"/>
-      <c r="B25" s="10">
+    <row r="25" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="11"/>
+      <c r="B25" s="5">
         <v>24</v>
       </c>
-      <c r="C25" s="11" t="s">
+      <c r="C25" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="D25" s="12">
+      <c r="D25" s="7">
         <v>1</v>
       </c>
-      <c r="E25" s="12"/>
-      <c r="F25" s="10" t="s">
+      <c r="E25" s="7"/>
+      <c r="F25" s="5" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="26" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="2"/>
-      <c r="B26" s="13">
+    <row r="26" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="11"/>
+      <c r="B26" s="8">
         <v>25</v>
       </c>
-      <c r="C26" s="14" t="s">
+      <c r="C26" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="D26" s="15"/>
-      <c r="E26" s="15"/>
+      <c r="D26" s="10"/>
+      <c r="E26" s="10"/>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A27" s="2"/>
+      <c r="A27" s="11"/>
       <c r="B27">
         <v>26</v>
       </c>
-      <c r="C27" s="6" t="s">
+      <c r="C27" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D27" s="7">
+      <c r="D27" s="3">
         <v>0</v>
       </c>
       <c r="I27" t="s">
@@ -1318,14 +1321,14 @@
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A28" s="2"/>
+      <c r="A28" s="11"/>
       <c r="B28">
         <v>27</v>
       </c>
-      <c r="C28" s="6" t="s">
+      <c r="C28" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D28" s="7">
+      <c r="D28" s="3">
         <v>1</v>
       </c>
       <c r="I28" t="s">
@@ -1333,14 +1336,14 @@
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A29" s="2"/>
+      <c r="A29" s="11"/>
       <c r="B29">
         <v>28</v>
       </c>
-      <c r="C29" s="6" t="s">
+      <c r="C29" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D29" s="7">
+      <c r="D29" s="3">
         <v>2</v>
       </c>
       <c r="I29" t="s">
@@ -1348,105 +1351,105 @@
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A30" s="2"/>
+      <c r="A30" s="11"/>
       <c r="B30">
         <v>29</v>
       </c>
-      <c r="C30" s="6" t="s">
+      <c r="C30" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D30" s="7">
+      <c r="D30" s="3">
         <v>3</v>
       </c>
       <c r="I30" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="31" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="2"/>
-      <c r="B31" s="13">
+    <row r="31" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="11"/>
+      <c r="B31" s="8">
         <v>30</v>
       </c>
-      <c r="C31" s="14" t="s">
+      <c r="C31" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="D31" s="15"/>
-      <c r="E31" s="15"/>
-    </row>
-    <row r="32" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="2"/>
-      <c r="B32" s="13">
+      <c r="D31" s="10"/>
+      <c r="E31" s="10"/>
+    </row>
+    <row r="32" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="11"/>
+      <c r="B32" s="8">
         <v>31</v>
       </c>
-      <c r="C32" s="14" t="s">
+      <c r="C32" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="D32" s="15"/>
-      <c r="E32" s="15"/>
-    </row>
-    <row r="33" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="2"/>
-      <c r="B33" s="13">
+      <c r="D32" s="10"/>
+      <c r="E32" s="10"/>
+    </row>
+    <row r="33" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="11"/>
+      <c r="B33" s="8">
         <v>32</v>
       </c>
-      <c r="C33" s="14" t="s">
+      <c r="C33" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="D33" s="15"/>
-      <c r="E33" s="15"/>
-    </row>
-    <row r="34" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="2"/>
-      <c r="B34" s="13">
+      <c r="D33" s="10"/>
+      <c r="E33" s="10"/>
+    </row>
+    <row r="34" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="11"/>
+      <c r="B34" s="8">
         <v>33</v>
       </c>
-      <c r="C34" s="14" t="s">
+      <c r="C34" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="D34" s="15"/>
-      <c r="E34" s="15"/>
-    </row>
-    <row r="35" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="2"/>
-      <c r="B35" s="10">
+      <c r="D34" s="10"/>
+      <c r="E34" s="10"/>
+    </row>
+    <row r="35" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="11"/>
+      <c r="B35" s="5">
         <v>34</v>
       </c>
-      <c r="C35" s="11" t="s">
+      <c r="C35" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="D35" s="12">
+      <c r="D35" s="7">
         <v>0</v>
       </c>
-      <c r="E35" s="12"/>
-      <c r="F35" s="10" t="s">
+      <c r="E35" s="7"/>
+      <c r="F35" s="5" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="36" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="2"/>
-      <c r="B36" s="10">
+    <row r="36" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="11"/>
+      <c r="B36" s="5">
         <v>35</v>
       </c>
-      <c r="C36" s="11" t="s">
+      <c r="C36" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="D36" s="12">
+      <c r="D36" s="7">
         <v>1</v>
       </c>
-      <c r="E36" s="12"/>
-      <c r="F36" s="10" t="s">
+      <c r="E36" s="7"/>
+      <c r="F36" s="5" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A37" s="2"/>
+      <c r="A37" s="11"/>
       <c r="B37">
         <v>36</v>
       </c>
-      <c r="C37" s="6" t="s">
+      <c r="C37" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D37" s="7">
+      <c r="D37" s="3">
         <v>2</v>
       </c>
       <c r="H37" t="s">
@@ -1457,16 +1460,16 @@
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A38" s="3" t="s">
+      <c r="A38" s="12" t="s">
         <v>3</v>
       </c>
       <c r="B38">
         <v>37</v>
       </c>
-      <c r="C38" s="6" t="s">
+      <c r="C38" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D38" s="7">
+      <c r="D38" s="3">
         <v>3</v>
       </c>
       <c r="H38" t="s">
@@ -1476,100 +1479,100 @@
         <v>95</v>
       </c>
     </row>
-    <row r="39" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="3"/>
-      <c r="B39" s="13">
+    <row r="39" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="12"/>
+      <c r="B39" s="8">
         <v>38</v>
       </c>
-      <c r="C39" s="14" t="s">
+      <c r="C39" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="D39" s="15"/>
-      <c r="E39" s="15"/>
-    </row>
-    <row r="40" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="3"/>
-      <c r="B40" s="13">
+      <c r="D39" s="10"/>
+      <c r="E39" s="10"/>
+    </row>
+    <row r="40" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="12"/>
+      <c r="B40" s="8">
         <v>39</v>
       </c>
-      <c r="C40" s="14" t="s">
+      <c r="C40" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="D40" s="15"/>
-      <c r="E40" s="15"/>
+      <c r="D40" s="10"/>
+      <c r="E40" s="10"/>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A41" s="3"/>
+      <c r="A41" s="12"/>
       <c r="B41">
         <v>40</v>
       </c>
-      <c r="C41" s="6" t="s">
+      <c r="C41" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D41" s="7">
+      <c r="D41" s="3">
         <v>4</v>
       </c>
       <c r="I41" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="42" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="3"/>
-      <c r="B42" s="10">
+    <row r="42" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="12"/>
+      <c r="B42" s="5">
         <v>41</v>
       </c>
-      <c r="C42" s="11" t="s">
+      <c r="C42" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="D42" s="12">
+      <c r="D42" s="7">
         <v>5</v>
       </c>
-      <c r="E42" s="12"/>
-      <c r="F42" s="10" t="s">
+      <c r="E42" s="7"/>
+      <c r="F42" s="5" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="43" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="3"/>
-      <c r="B43" s="10">
+    <row r="43" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="12"/>
+      <c r="B43" s="5">
         <v>42</v>
       </c>
-      <c r="C43" s="11" t="s">
+      <c r="C43" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="D43" s="12">
+      <c r="D43" s="7">
         <v>6</v>
       </c>
-      <c r="E43" s="12"/>
-      <c r="F43" s="10" t="s">
+      <c r="E43" s="7"/>
+      <c r="F43" s="5" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="44" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="3"/>
-      <c r="B44" s="10">
+    <row r="44" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="12"/>
+      <c r="B44" s="5">
         <v>43</v>
       </c>
-      <c r="C44" s="11" t="s">
+      <c r="C44" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="D44" s="12">
+      <c r="D44" s="7">
         <v>7</v>
       </c>
-      <c r="E44" s="12"/>
-      <c r="F44" s="10" t="s">
+      <c r="E44" s="7"/>
+      <c r="F44" s="5" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A45" s="3"/>
+      <c r="A45" s="12"/>
       <c r="B45">
         <v>44</v>
       </c>
-      <c r="C45" s="6" t="s">
+      <c r="C45" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D45" s="7">
+      <c r="D45" s="3">
         <v>4</v>
       </c>
       <c r="I45" t="s">
@@ -1577,252 +1580,252 @@
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A46" s="3"/>
+      <c r="A46" s="12"/>
       <c r="B46">
         <v>45</v>
       </c>
-      <c r="C46" s="6" t="s">
+      <c r="C46" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D46" s="7">
+      <c r="D46" s="3">
         <v>5</v>
       </c>
       <c r="I46" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="47" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="3"/>
-      <c r="B47" s="10">
+    <row r="47" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="12"/>
+      <c r="B47" s="5">
         <v>46</v>
       </c>
-      <c r="C47" s="11" t="s">
+      <c r="C47" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="D47" s="12">
+      <c r="D47" s="7">
         <v>0</v>
       </c>
-      <c r="E47" s="12"/>
-      <c r="F47" s="10" t="s">
+      <c r="E47" s="7"/>
+      <c r="F47" s="5" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="48" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="3"/>
-      <c r="B48" s="10">
+    <row r="48" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="12"/>
+      <c r="B48" s="5">
         <v>47</v>
       </c>
-      <c r="C48" s="11" t="s">
+      <c r="C48" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="D48" s="12">
+      <c r="D48" s="7">
         <v>1</v>
       </c>
-      <c r="E48" s="12"/>
-      <c r="F48" s="10" t="s">
+      <c r="E48" s="7"/>
+      <c r="F48" s="5" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="49" spans="1:8" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="3"/>
-      <c r="B49" s="10">
+    <row r="49" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="12"/>
+      <c r="B49" s="5">
         <v>48</v>
       </c>
-      <c r="C49" s="11" t="s">
+      <c r="C49" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="D49" s="12">
+      <c r="D49" s="7">
         <v>2</v>
       </c>
-      <c r="E49" s="12"/>
-      <c r="F49" s="10" t="s">
+      <c r="E49" s="7"/>
+      <c r="F49" s="5" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A50" s="3"/>
+      <c r="A50" s="12"/>
       <c r="B50">
         <v>49</v>
       </c>
-      <c r="C50" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="D50" s="7">
+      <c r="C50" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D50" s="3">
         <v>11</v>
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A51" s="3"/>
+      <c r="A51" s="12"/>
       <c r="B51">
         <v>50</v>
       </c>
-      <c r="C51" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="D51" s="7">
+      <c r="C51" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D51" s="3">
         <v>12</v>
       </c>
     </row>
-    <row r="52" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="3"/>
-      <c r="B52" s="13">
+    <row r="52" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="12"/>
+      <c r="B52" s="8">
         <v>51</v>
       </c>
-      <c r="C52" s="14" t="s">
+      <c r="C52" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="D52" s="15"/>
-      <c r="E52" s="15"/>
-    </row>
-    <row r="53" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="3"/>
-      <c r="B53" s="13">
+      <c r="D52" s="10"/>
+      <c r="E52" s="10"/>
+    </row>
+    <row r="53" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="12"/>
+      <c r="B53" s="8">
         <v>52</v>
       </c>
-      <c r="C53" s="14" t="s">
+      <c r="C53" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="D53" s="15"/>
-      <c r="E53" s="15"/>
+      <c r="D53" s="10"/>
+      <c r="E53" s="10"/>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A54" s="3"/>
+      <c r="A54" s="12"/>
       <c r="B54">
         <v>53</v>
       </c>
-      <c r="C54" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="D54" s="7">
+      <c r="C54" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D54" s="3">
         <v>13</v>
       </c>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A55" s="3"/>
+      <c r="A55" s="12"/>
       <c r="B55">
         <v>54</v>
       </c>
-      <c r="C55" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="D55" s="7">
+      <c r="C55" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D55" s="3">
         <v>14</v>
       </c>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A56" s="3"/>
+      <c r="A56" s="12"/>
       <c r="B56">
         <v>55</v>
       </c>
-      <c r="C56" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="D56" s="7">
+      <c r="C56" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D56" s="3">
         <v>15</v>
       </c>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A57" s="3"/>
+      <c r="A57" s="12"/>
       <c r="B57">
         <v>56</v>
       </c>
-      <c r="C57" s="6" t="s">
+      <c r="C57" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D57" s="7">
+      <c r="D57" s="3">
         <v>0</v>
       </c>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A58" s="3"/>
+      <c r="A58" s="12"/>
       <c r="B58">
         <v>57</v>
       </c>
-      <c r="C58" s="6" t="s">
+      <c r="C58" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D58" s="7">
+      <c r="D58" s="3">
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="1:8" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="3"/>
-      <c r="B59" s="10">
+    <row r="59" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A59" s="12"/>
+      <c r="B59" s="5">
         <v>58</v>
       </c>
-      <c r="C59" s="11" t="s">
+      <c r="C59" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="D59" s="12">
+      <c r="D59" s="7">
         <v>7</v>
       </c>
-      <c r="E59" s="12"/>
-      <c r="F59" s="10" t="s">
+      <c r="E59" s="7"/>
+      <c r="F59" s="5" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="60" spans="1:8" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="3"/>
-      <c r="B60" s="10">
+    <row r="60" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A60" s="12"/>
+      <c r="B60" s="5">
         <v>59</v>
       </c>
-      <c r="C60" s="11" t="s">
+      <c r="C60" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="D60" s="12">
+      <c r="D60" s="7">
         <v>8</v>
       </c>
-      <c r="E60" s="12"/>
-      <c r="F60" s="10" t="s">
+      <c r="E60" s="7"/>
+      <c r="F60" s="5" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A61" s="3"/>
+      <c r="A61" s="12"/>
       <c r="B61">
         <v>60</v>
       </c>
-      <c r="C61" s="6" t="s">
+      <c r="C61" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D61" s="7">
+      <c r="D61" s="3">
         <v>9</v>
       </c>
       <c r="H61" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="62" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="3"/>
-      <c r="B62" s="13">
+    <row r="62" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A62" s="12"/>
+      <c r="B62" s="8">
         <v>61</v>
       </c>
-      <c r="C62" s="14" t="s">
+      <c r="C62" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="D62" s="15"/>
-      <c r="E62" s="15"/>
-    </row>
-    <row r="63" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="3"/>
-      <c r="B63" s="13">
+      <c r="D62" s="10"/>
+      <c r="E62" s="10"/>
+    </row>
+    <row r="63" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A63" s="12"/>
+      <c r="B63" s="8">
         <v>62</v>
       </c>
-      <c r="C63" s="14" t="s">
+      <c r="C63" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="D63" s="15"/>
-      <c r="E63" s="15"/>
+      <c r="D63" s="10"/>
+      <c r="E63" s="10"/>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A64" s="3"/>
+      <c r="A64" s="12"/>
       <c r="B64">
         <v>63</v>
       </c>
-      <c r="C64" s="6" t="s">
+      <c r="C64" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D64" s="7">
+      <c r="D64" s="3">
         <v>10</v>
       </c>
       <c r="H64" t="s">
@@ -1830,268 +1833,268 @@
       </c>
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A65" s="3"/>
+      <c r="A65" s="12"/>
       <c r="B65">
         <v>64</v>
       </c>
-      <c r="C65" s="6" t="s">
+      <c r="C65" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D65" s="7">
+      <c r="D65" s="3">
         <v>11</v>
       </c>
       <c r="H65" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="66" spans="1:8" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="3"/>
-      <c r="B66" s="10">
+    <row r="66" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A66" s="12"/>
+      <c r="B66" s="5">
         <v>65</v>
       </c>
-      <c r="C66" s="11" t="s">
+      <c r="C66" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="D66" s="12">
+      <c r="D66" s="7">
         <v>12</v>
       </c>
-      <c r="E66" s="12"/>
-      <c r="F66" s="10" t="s">
+      <c r="E66" s="7"/>
+      <c r="F66" s="5" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="67" spans="1:8" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="3"/>
-      <c r="B67" s="10">
+    <row r="67" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A67" s="12"/>
+      <c r="B67" s="5">
         <v>66</v>
       </c>
-      <c r="C67" s="11" t="s">
+      <c r="C67" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="D67" s="12">
+      <c r="D67" s="7">
         <v>13</v>
       </c>
-      <c r="E67" s="12"/>
-      <c r="F67" s="10" t="s">
+      <c r="E67" s="7"/>
+      <c r="F67" s="5" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="68" spans="1:8" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="3"/>
-      <c r="B68" s="10">
+    <row r="68" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A68" s="12"/>
+      <c r="B68" s="5">
         <v>67</v>
       </c>
-      <c r="C68" s="11" t="s">
+      <c r="C68" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="D68" s="12">
+      <c r="D68" s="7">
         <v>14</v>
       </c>
-      <c r="E68" s="12"/>
-      <c r="F68" s="10" t="s">
+      <c r="E68" s="7"/>
+      <c r="F68" s="5" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A69" s="3"/>
+      <c r="A69" s="12"/>
       <c r="B69">
         <v>68</v>
       </c>
-      <c r="C69" s="6" t="s">
+      <c r="C69" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D69" s="7">
+      <c r="D69" s="3">
         <v>15</v>
       </c>
     </row>
-    <row r="70" spans="1:8" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="3"/>
-      <c r="B70" s="10">
+    <row r="70" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A70" s="12"/>
+      <c r="B70" s="5">
         <v>69</v>
       </c>
-      <c r="C70" s="11" t="s">
+      <c r="C70" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="D70" s="12">
+      <c r="D70" s="7">
         <v>10</v>
       </c>
-      <c r="E70" s="12"/>
-      <c r="F70" s="10" t="s">
+      <c r="E70" s="7"/>
+      <c r="F70" s="5" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="71" spans="1:8" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="3"/>
-      <c r="B71" s="10">
+    <row r="71" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A71" s="12"/>
+      <c r="B71" s="5">
         <v>70</v>
       </c>
-      <c r="C71" s="11" t="s">
+      <c r="C71" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="D71" s="12">
+      <c r="D71" s="7">
         <v>11</v>
       </c>
-      <c r="E71" s="12"/>
-      <c r="F71" s="10" t="s">
+      <c r="E71" s="7"/>
+      <c r="F71" s="5" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="72" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="3"/>
-      <c r="B72" s="13">
+    <row r="72" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A72" s="12"/>
+      <c r="B72" s="8">
         <v>71</v>
       </c>
-      <c r="C72" s="14" t="s">
+      <c r="C72" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="D72" s="15"/>
-      <c r="E72" s="15"/>
-    </row>
-    <row r="73" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="3"/>
-      <c r="B73" s="13">
+      <c r="D72" s="10"/>
+      <c r="E72" s="10"/>
+    </row>
+    <row r="73" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A73" s="12"/>
+      <c r="B73" s="8">
         <v>72</v>
       </c>
-      <c r="C73" s="14" t="s">
+      <c r="C73" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="D73" s="15"/>
-      <c r="E73" s="15"/>
-    </row>
-    <row r="74" spans="1:8" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="4" t="s">
+      <c r="D73" s="10"/>
+      <c r="E73" s="10"/>
+    </row>
+    <row r="74" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A74" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="B74" s="10">
+      <c r="B74" s="5">
         <v>73</v>
       </c>
-      <c r="C74" s="11" t="s">
+      <c r="C74" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="D74" s="12">
+      <c r="D74" s="7">
         <v>12</v>
       </c>
-      <c r="E74" s="12"/>
-      <c r="F74" s="10" t="s">
+      <c r="E74" s="7"/>
+      <c r="F74" s="5" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="75" spans="1:8" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="4"/>
-      <c r="B75" s="10">
+    <row r="75" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A75" s="13"/>
+      <c r="B75" s="5">
         <v>74</v>
       </c>
-      <c r="C75" s="11" t="s">
+      <c r="C75" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="D75" s="12">
+      <c r="D75" s="7">
         <v>13</v>
       </c>
-      <c r="E75" s="12"/>
-      <c r="F75" s="10" t="s">
+      <c r="E75" s="7"/>
+      <c r="F75" s="5" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="76" spans="1:8" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A76" s="4"/>
-      <c r="B76" s="10">
+    <row r="76" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A76" s="13"/>
+      <c r="B76" s="5">
         <v>75</v>
       </c>
-      <c r="C76" s="11" t="s">
+      <c r="C76" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="D76" s="12">
+      <c r="D76" s="7">
         <v>14</v>
       </c>
-      <c r="E76" s="12"/>
-      <c r="F76" s="10" t="s">
+      <c r="E76" s="7"/>
+      <c r="F76" s="5" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A77" s="4"/>
+      <c r="A77" s="13"/>
       <c r="B77">
         <v>76</v>
       </c>
-      <c r="C77" s="6" t="s">
+      <c r="C77" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D77" s="7">
+      <c r="D77" s="3">
         <v>15</v>
       </c>
       <c r="H77" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="78" spans="1:8" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A78" s="4"/>
-      <c r="B78" s="10">
+    <row r="78" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A78" s="13"/>
+      <c r="B78" s="5">
         <v>77</v>
       </c>
-      <c r="C78" s="11" t="s">
+      <c r="C78" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="D78" s="12">
+      <c r="D78" s="7">
         <v>8</v>
       </c>
-      <c r="E78" s="12"/>
-      <c r="F78" s="10" t="s">
+      <c r="E78" s="7"/>
+      <c r="F78" s="5" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="79" spans="1:8" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A79" s="4"/>
-      <c r="B79" s="10">
+    <row r="79" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A79" s="13"/>
+      <c r="B79" s="5">
         <v>78</v>
       </c>
-      <c r="C79" s="11" t="s">
+      <c r="C79" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="D79" s="12">
-        <v>9</v>
-      </c>
-      <c r="E79" s="12"/>
-      <c r="F79" s="10" t="s">
+      <c r="D79" s="7">
+        <v>9</v>
+      </c>
+      <c r="E79" s="7"/>
+      <c r="F79" s="5" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A80" s="4"/>
+      <c r="A80" s="13"/>
       <c r="B80">
         <v>79</v>
       </c>
-      <c r="C80" s="6" t="s">
+      <c r="C80" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="D80" s="7">
+      <c r="D80" s="3">
         <v>10</v>
       </c>
     </row>
-    <row r="81" spans="1:8" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A81" s="4"/>
-      <c r="B81" s="10">
+    <row r="81" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A81" s="13"/>
+      <c r="B81" s="5">
         <v>80</v>
       </c>
-      <c r="C81" s="11" t="s">
+      <c r="C81" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="D81" s="12">
+      <c r="D81" s="7">
         <v>11</v>
       </c>
-      <c r="E81" s="12"/>
-      <c r="F81" s="10" t="s">
+      <c r="E81" s="7"/>
+      <c r="F81" s="5" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="82" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A82" s="4"/>
+      <c r="A82" s="13"/>
       <c r="B82">
         <v>81</v>
       </c>
-      <c r="C82" s="6" t="s">
+      <c r="C82" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="D82" s="7">
+      <c r="D82" s="3">
         <v>12</v>
       </c>
       <c r="H82" t="s">
@@ -2099,51 +2102,51 @@
       </c>
     </row>
     <row r="83" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A83" s="4"/>
+      <c r="A83" s="13"/>
       <c r="B83">
         <v>82</v>
       </c>
-      <c r="C83" s="6" t="s">
+      <c r="C83" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="D83" s="7">
+      <c r="D83" s="3">
         <v>13</v>
       </c>
       <c r="H83" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="84" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A84" s="4"/>
-      <c r="B84" s="13">
+    <row r="84" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A84" s="13"/>
+      <c r="B84" s="8">
         <v>83</v>
       </c>
-      <c r="C84" s="14" t="s">
+      <c r="C84" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="D84" s="15"/>
-      <c r="E84" s="15"/>
-    </row>
-    <row r="85" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A85" s="4"/>
-      <c r="B85" s="13">
+      <c r="D84" s="10"/>
+      <c r="E84" s="10"/>
+    </row>
+    <row r="85" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A85" s="13"/>
+      <c r="B85" s="8">
         <v>84</v>
       </c>
-      <c r="C85" s="14" t="s">
+      <c r="C85" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="D85" s="15"/>
-      <c r="E85" s="15"/>
+      <c r="D85" s="10"/>
+      <c r="E85" s="10"/>
     </row>
     <row r="86" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A86" s="4"/>
+      <c r="A86" s="13"/>
       <c r="B86">
         <v>85</v>
       </c>
-      <c r="C86" s="6" t="s">
+      <c r="C86" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="D86" s="7">
+      <c r="D86" s="3">
         <v>14</v>
       </c>
       <c r="H86" t="s">
@@ -2151,14 +2154,14 @@
       </c>
     </row>
     <row r="87" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A87" s="4"/>
+      <c r="A87" s="13"/>
       <c r="B87">
         <v>86</v>
       </c>
-      <c r="C87" s="6" t="s">
+      <c r="C87" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="D87" s="7">
+      <c r="D87" s="3">
         <v>15</v>
       </c>
       <c r="H87" t="s">
@@ -2166,120 +2169,120 @@
       </c>
     </row>
     <row r="88" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A88" s="4"/>
+      <c r="A88" s="13"/>
       <c r="B88">
         <v>87</v>
       </c>
-      <c r="C88" s="6" t="s">
+      <c r="C88" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D88" s="7">
+      <c r="D88" s="3">
         <v>2</v>
       </c>
     </row>
     <row r="89" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A89" s="4"/>
+      <c r="A89" s="13"/>
       <c r="B89">
         <v>88</v>
       </c>
-      <c r="C89" s="6" t="s">
+      <c r="C89" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D89" s="7">
+      <c r="D89" s="3">
         <v>3</v>
       </c>
     </row>
     <row r="90" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A90" s="4"/>
+      <c r="A90" s="13"/>
       <c r="B90">
         <v>89</v>
       </c>
-      <c r="C90" s="6" t="s">
+      <c r="C90" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D90" s="7">
+      <c r="D90" s="3">
         <v>4</v>
       </c>
     </row>
     <row r="91" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A91" s="4"/>
+      <c r="A91" s="13"/>
       <c r="B91">
         <v>90</v>
       </c>
-      <c r="C91" s="6" t="s">
+      <c r="C91" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D91" s="7">
+      <c r="D91" s="3">
         <v>5</v>
       </c>
     </row>
     <row r="92" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A92" s="4"/>
+      <c r="A92" s="13"/>
       <c r="B92">
         <v>91</v>
       </c>
-      <c r="C92" s="6" t="s">
+      <c r="C92" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D92" s="7">
+      <c r="D92" s="3">
         <v>6</v>
       </c>
     </row>
     <row r="93" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A93" s="4"/>
+      <c r="A93" s="13"/>
       <c r="B93">
         <v>92</v>
       </c>
-      <c r="C93" s="6" t="s">
+      <c r="C93" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D93" s="7">
+      <c r="D93" s="3">
         <v>7</v>
       </c>
     </row>
     <row r="94" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A94" s="4"/>
+      <c r="A94" s="13"/>
       <c r="B94">
         <v>93</v>
       </c>
-      <c r="C94" s="6" t="s">
+      <c r="C94" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D94" s="7">
+      <c r="D94" s="3">
         <v>8</v>
       </c>
     </row>
-    <row r="95" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A95" s="4"/>
-      <c r="B95" s="13">
+    <row r="95" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A95" s="13"/>
+      <c r="B95" s="8">
         <v>94</v>
       </c>
-      <c r="C95" s="14" t="s">
+      <c r="C95" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="D95" s="15"/>
-      <c r="E95" s="15"/>
-    </row>
-    <row r="96" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A96" s="4"/>
-      <c r="B96" s="13">
+      <c r="D95" s="10"/>
+      <c r="E95" s="10"/>
+    </row>
+    <row r="96" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A96" s="13"/>
+      <c r="B96" s="8">
         <v>95</v>
       </c>
-      <c r="C96" s="14" t="s">
+      <c r="C96" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="D96" s="15"/>
-      <c r="E96" s="15"/>
+      <c r="D96" s="10"/>
+      <c r="E96" s="10"/>
     </row>
     <row r="97" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A97" s="4"/>
+      <c r="A97" s="13"/>
       <c r="B97">
         <v>96</v>
       </c>
-      <c r="C97" s="6" t="s">
+      <c r="C97" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D97" s="7">
+      <c r="D97" s="3">
         <v>6</v>
       </c>
       <c r="H97" t="s">
@@ -2287,532 +2290,532 @@
       </c>
     </row>
     <row r="98" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A98" s="4"/>
+      <c r="A98" s="13"/>
       <c r="B98">
         <v>97</v>
       </c>
-      <c r="C98" s="6" t="s">
+      <c r="C98" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D98" s="7">
+      <c r="D98" s="3">
         <v>7</v>
       </c>
       <c r="H98" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="99" spans="1:8" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A99" s="4"/>
-      <c r="B99" s="10">
+    <row r="99" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A99" s="13"/>
+      <c r="B99" s="5">
         <v>98</v>
       </c>
-      <c r="C99" s="11" t="s">
+      <c r="C99" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="D99" s="12">
+      <c r="D99" s="7">
         <v>8</v>
       </c>
-      <c r="E99" s="12"/>
-      <c r="F99" s="10" t="s">
+      <c r="E99" s="7"/>
+      <c r="F99" s="5" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="100" spans="1:8" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A100" s="4"/>
-      <c r="B100" s="10">
+    <row r="100" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A100" s="13"/>
+      <c r="B100" s="5">
         <v>99</v>
       </c>
-      <c r="C100" s="11" t="s">
+      <c r="C100" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="D100" s="12">
-        <v>9</v>
-      </c>
-      <c r="E100" s="12"/>
-      <c r="F100" s="10" t="s">
+      <c r="D100" s="7">
+        <v>9</v>
+      </c>
+      <c r="E100" s="7"/>
+      <c r="F100" s="5" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="101" spans="1:8" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A101" s="4"/>
-      <c r="B101" s="10">
+    <row r="101" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A101" s="13"/>
+      <c r="B101" s="5">
         <v>100</v>
       </c>
-      <c r="C101" s="11" t="s">
+      <c r="C101" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="D101" s="12">
+      <c r="D101" s="7">
         <v>8</v>
       </c>
-      <c r="E101" s="12"/>
-      <c r="F101" s="10" t="s">
+      <c r="E101" s="7"/>
+      <c r="F101" s="5" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="102" spans="1:8" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A102" s="4"/>
-      <c r="B102" s="10">
+    <row r="102" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A102" s="13"/>
+      <c r="B102" s="5">
         <v>101</v>
       </c>
-      <c r="C102" s="11" t="s">
+      <c r="C102" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="D102" s="12">
-        <v>9</v>
-      </c>
-      <c r="E102" s="12"/>
-      <c r="F102" s="10" t="s">
+      <c r="D102" s="7">
+        <v>9</v>
+      </c>
+      <c r="E102" s="7"/>
+      <c r="F102" s="5" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="103" spans="1:8" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A103" s="4"/>
-      <c r="B103" s="10">
+    <row r="103" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A103" s="13"/>
+      <c r="B103" s="5">
         <v>102</v>
       </c>
-      <c r="C103" s="11" t="s">
+      <c r="C103" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="D103" s="12">
+      <c r="D103" s="7">
         <v>10</v>
       </c>
-      <c r="E103" s="12"/>
-      <c r="F103" s="10" t="s">
+      <c r="E103" s="7"/>
+      <c r="F103" s="5" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="104" spans="1:8" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A104" s="4"/>
-      <c r="B104" s="10">
+    <row r="104" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A104" s="13"/>
+      <c r="B104" s="5">
         <v>103</v>
       </c>
-      <c r="C104" s="11" t="s">
+      <c r="C104" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="D104" s="12">
+      <c r="D104" s="7">
         <v>11</v>
       </c>
-      <c r="E104" s="12"/>
-      <c r="F104" s="10" t="s">
+      <c r="E104" s="7"/>
+      <c r="F104" s="5" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="105" spans="1:8" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A105" s="4"/>
-      <c r="B105" s="10">
+    <row r="105" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A105" s="13"/>
+      <c r="B105" s="5">
         <v>104</v>
       </c>
-      <c r="C105" s="11" t="s">
+      <c r="C105" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="D105" s="12">
+      <c r="D105" s="7">
         <v>12</v>
       </c>
-      <c r="E105" s="12"/>
-      <c r="F105" s="10" t="s">
+      <c r="E105" s="7"/>
+      <c r="F105" s="5" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="106" spans="1:8" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A106" s="4"/>
-      <c r="B106" s="10">
+    <row r="106" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A106" s="13"/>
+      <c r="B106" s="5">
         <v>105</v>
       </c>
-      <c r="C106" s="11" t="s">
+      <c r="C106" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="D106" s="12">
+      <c r="D106" s="7">
         <v>13</v>
       </c>
-      <c r="E106" s="12"/>
-      <c r="F106" s="10" t="s">
+      <c r="E106" s="7"/>
+      <c r="F106" s="5" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="107" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A107" s="4"/>
-      <c r="B107" s="13">
+    <row r="107" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A107" s="13"/>
+      <c r="B107" s="8">
         <v>106</v>
       </c>
-      <c r="C107" s="14" t="s">
+      <c r="C107" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="D107" s="15"/>
-      <c r="E107" s="15"/>
-    </row>
-    <row r="108" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A108" s="4"/>
-      <c r="B108" s="13">
+      <c r="D107" s="10"/>
+      <c r="E107" s="10"/>
+    </row>
+    <row r="108" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A108" s="13"/>
+      <c r="B108" s="8">
         <v>107</v>
       </c>
-      <c r="C108" s="14" t="s">
+      <c r="C108" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="D108" s="15"/>
-      <c r="E108" s="15"/>
-    </row>
-    <row r="109" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A109" s="4"/>
-      <c r="B109" s="13">
+      <c r="D108" s="10"/>
+      <c r="E108" s="10"/>
+    </row>
+    <row r="109" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A109" s="13"/>
+      <c r="B109" s="8">
         <v>108</v>
       </c>
-      <c r="C109" s="14" t="s">
+      <c r="C109" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="D109" s="15"/>
-      <c r="E109" s="15"/>
-    </row>
-    <row r="110" spans="1:8" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A110" s="5" t="s">
+      <c r="D109" s="10"/>
+      <c r="E109" s="10"/>
+    </row>
+    <row r="110" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A110" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="B110" s="10">
+      <c r="B110" s="5">
         <v>109</v>
       </c>
-      <c r="C110" s="11" t="s">
+      <c r="C110" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="D110" s="12">
+      <c r="D110" s="7">
         <v>14</v>
       </c>
-      <c r="E110" s="12"/>
-      <c r="F110" s="10" t="s">
+      <c r="E110" s="7"/>
+      <c r="F110" s="5" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="111" spans="1:8" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A111" s="5"/>
-      <c r="B111" s="10">
+    <row r="111" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A111" s="14"/>
+      <c r="B111" s="5">
         <v>110</v>
       </c>
-      <c r="C111" s="11" t="s">
+      <c r="C111" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="D111" s="12">
+      <c r="D111" s="7">
         <v>15</v>
       </c>
-      <c r="E111" s="12"/>
-      <c r="F111" s="10" t="s">
+      <c r="E111" s="7"/>
+      <c r="F111" s="5" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="112" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A112" s="5"/>
+      <c r="A112" s="14"/>
       <c r="B112">
         <v>111</v>
       </c>
-      <c r="C112" s="6" t="s">
+      <c r="C112" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D112" s="7">
+      <c r="D112" s="3">
         <v>10</v>
       </c>
     </row>
-    <row r="113" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A113" s="5"/>
-      <c r="B113" s="10">
+    <row r="113" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A113" s="14"/>
+      <c r="B113" s="5">
         <v>112</v>
       </c>
-      <c r="C113" s="11" t="s">
+      <c r="C113" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="D113" s="12">
+      <c r="D113" s="7">
         <v>11</v>
       </c>
-      <c r="E113" s="12"/>
-      <c r="F113" s="10" t="s">
+      <c r="E113" s="7"/>
+      <c r="F113" s="5" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="114" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A114" s="5"/>
+      <c r="A114" s="14"/>
       <c r="B114">
         <v>113</v>
       </c>
-      <c r="C114" s="6" t="s">
+      <c r="C114" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D114" s="7">
+      <c r="D114" s="3">
         <v>12</v>
       </c>
     </row>
-    <row r="115" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A115" s="5"/>
-      <c r="B115" s="10">
+    <row r="115" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A115" s="14"/>
+      <c r="B115" s="5">
         <v>114</v>
       </c>
-      <c r="C115" s="11" t="s">
+      <c r="C115" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="D115" s="12">
+      <c r="D115" s="7">
         <v>0</v>
       </c>
-      <c r="E115" s="12"/>
-      <c r="F115" s="10" t="s">
+      <c r="E115" s="7"/>
+      <c r="F115" s="5" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="116" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A116" s="5"/>
-      <c r="B116" s="10">
+    <row r="116" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A116" s="14"/>
+      <c r="B116" s="5">
         <v>115</v>
       </c>
-      <c r="C116" s="11" t="s">
+      <c r="C116" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="D116" s="12">
+      <c r="D116" s="7">
         <v>1</v>
       </c>
-      <c r="E116" s="12"/>
-      <c r="F116" s="10" t="s">
+      <c r="E116" s="7"/>
+      <c r="F116" s="5" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="117" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A117" s="5"/>
-      <c r="B117" s="10">
+    <row r="117" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A117" s="14"/>
+      <c r="B117" s="5">
         <v>116</v>
       </c>
-      <c r="C117" s="11" t="s">
+      <c r="C117" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="D117" s="12">
+      <c r="D117" s="7">
         <v>2</v>
       </c>
-      <c r="E117" s="12"/>
-      <c r="F117" s="10" t="s">
+      <c r="E117" s="7"/>
+      <c r="F117" s="5" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="118" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A118" s="5"/>
-      <c r="B118" s="10">
+    <row r="118" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A118" s="14"/>
+      <c r="B118" s="5">
         <v>117</v>
       </c>
-      <c r="C118" s="11" t="s">
+      <c r="C118" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="D118" s="12">
+      <c r="D118" s="7">
         <v>3</v>
       </c>
-      <c r="E118" s="12"/>
-      <c r="F118" s="10" t="s">
+      <c r="E118" s="7"/>
+      <c r="F118" s="5" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="119" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A119" s="5"/>
-      <c r="B119" s="10">
+    <row r="119" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A119" s="14"/>
+      <c r="B119" s="5">
         <v>118</v>
       </c>
-      <c r="C119" s="11" t="s">
+      <c r="C119" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="D119" s="12">
+      <c r="D119" s="7">
         <v>4</v>
       </c>
-      <c r="E119" s="12"/>
-      <c r="F119" s="10" t="s">
+      <c r="E119" s="7"/>
+      <c r="F119" s="5" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="120" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A120" s="5"/>
-      <c r="B120" s="10">
+    <row r="120" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A120" s="14"/>
+      <c r="B120" s="5">
         <v>119</v>
       </c>
-      <c r="C120" s="11" t="s">
+      <c r="C120" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="D120" s="12">
+      <c r="D120" s="7">
         <v>5</v>
       </c>
-      <c r="E120" s="12"/>
-      <c r="F120" s="10" t="s">
+      <c r="E120" s="7"/>
+      <c r="F120" s="5" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="121" spans="1:6" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A121" s="5"/>
-      <c r="B121" s="13">
+    <row r="121" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A121" s="14"/>
+      <c r="B121" s="8">
         <v>120</v>
       </c>
-      <c r="C121" s="14" t="s">
+      <c r="C121" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="D121" s="15"/>
-      <c r="E121" s="15"/>
-    </row>
-    <row r="122" spans="1:6" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A122" s="5"/>
-      <c r="B122" s="13">
+      <c r="D121" s="10"/>
+      <c r="E121" s="10"/>
+    </row>
+    <row r="122" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A122" s="14"/>
+      <c r="B122" s="8">
         <v>121</v>
       </c>
-      <c r="C122" s="14" t="s">
+      <c r="C122" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="D122" s="15"/>
-      <c r="E122" s="15"/>
-    </row>
-    <row r="123" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A123" s="5"/>
-      <c r="B123" s="10">
+      <c r="D122" s="10"/>
+      <c r="E122" s="10"/>
+    </row>
+    <row r="123" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A123" s="14"/>
+      <c r="B123" s="5">
         <v>122</v>
       </c>
-      <c r="C123" s="11" t="s">
+      <c r="C123" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="D123" s="12">
+      <c r="D123" s="7">
         <v>6</v>
       </c>
-      <c r="E123" s="12"/>
-      <c r="F123" s="10" t="s">
+      <c r="E123" s="7"/>
+      <c r="F123" s="5" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="124" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A124" s="5"/>
+      <c r="A124" s="14"/>
       <c r="B124">
         <v>123</v>
       </c>
-      <c r="C124" s="6" t="s">
+      <c r="C124" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="D124" s="7">
+      <c r="D124" s="3">
         <v>7</v>
       </c>
     </row>
     <row r="125" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A125" s="5"/>
+      <c r="A125" s="14"/>
       <c r="B125">
         <v>124</v>
       </c>
-      <c r="C125" s="6" t="s">
+      <c r="C125" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D125" s="7">
+      <c r="D125" s="3">
         <v>9</v>
       </c>
     </row>
     <row r="126" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A126" s="5"/>
+      <c r="A126" s="14"/>
       <c r="B126">
         <v>125</v>
       </c>
-      <c r="C126" s="6" t="s">
+      <c r="C126" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D126" s="7">
+      <c r="D126" s="3">
         <v>10</v>
       </c>
     </row>
     <row r="127" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A127" s="5"/>
+      <c r="A127" s="14"/>
       <c r="B127">
         <v>126</v>
       </c>
-      <c r="C127" s="6" t="s">
+      <c r="C127" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D127" s="7">
+      <c r="D127" s="3">
         <v>11</v>
       </c>
     </row>
     <row r="128" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A128" s="5"/>
+      <c r="A128" s="14"/>
       <c r="B128">
         <v>127</v>
       </c>
-      <c r="C128" s="6" t="s">
+      <c r="C128" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D128" s="7">
+      <c r="D128" s="3">
         <v>12</v>
       </c>
     </row>
     <row r="129" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A129" s="5"/>
+      <c r="A129" s="14"/>
       <c r="B129">
         <v>128</v>
       </c>
-      <c r="C129" s="6" t="s">
+      <c r="C129" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D129" s="7">
+      <c r="D129" s="3">
         <v>13</v>
       </c>
     </row>
     <row r="130" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A130" s="5"/>
+      <c r="A130" s="14"/>
       <c r="B130">
         <v>129</v>
       </c>
-      <c r="C130" s="6" t="s">
+      <c r="C130" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D130" s="7">
+      <c r="D130" s="3">
         <v>14</v>
       </c>
     </row>
-    <row r="131" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A131" s="5"/>
-      <c r="B131" s="13">
+    <row r="131" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A131" s="14"/>
+      <c r="B131" s="8">
         <v>130</v>
       </c>
-      <c r="C131" s="14" t="s">
+      <c r="C131" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="D131" s="15"/>
-      <c r="E131" s="15"/>
-    </row>
-    <row r="132" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A132" s="5"/>
-      <c r="B132" s="13">
+      <c r="D131" s="10"/>
+      <c r="E131" s="10"/>
+    </row>
+    <row r="132" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A132" s="14"/>
+      <c r="B132" s="8">
         <v>131</v>
       </c>
-      <c r="C132" s="14" t="s">
+      <c r="C132" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="D132" s="15"/>
-      <c r="E132" s="15"/>
+      <c r="D132" s="10"/>
+      <c r="E132" s="10"/>
     </row>
     <row r="133" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A133" s="5"/>
+      <c r="A133" s="14"/>
       <c r="B133">
         <v>132</v>
       </c>
-      <c r="C133" s="6" t="s">
+      <c r="C133" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D133" s="7">
+      <c r="D133" s="3">
         <v>15</v>
       </c>
     </row>
-    <row r="134" spans="1:8" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A134" s="5"/>
-      <c r="B134" s="10">
+    <row r="134" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A134" s="14"/>
+      <c r="B134" s="5">
         <v>133</v>
       </c>
-      <c r="C134" s="11" t="s">
+      <c r="C134" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="D134" s="12">
+      <c r="D134" s="7">
         <v>3</v>
       </c>
-      <c r="E134" s="12"/>
-      <c r="F134" s="10" t="s">
+      <c r="E134" s="7"/>
+      <c r="F134" s="5" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="135" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A135" s="5"/>
+      <c r="A135" s="14"/>
       <c r="B135">
         <v>134</v>
       </c>
-      <c r="C135" s="6" t="s">
+      <c r="C135" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D135" s="7">
+      <c r="D135" s="3">
         <v>4</v>
       </c>
       <c r="H135" t="s">
@@ -2820,74 +2823,74 @@
       </c>
     </row>
     <row r="136" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A136" s="5"/>
+      <c r="A136" s="14"/>
       <c r="B136">
         <v>135</v>
       </c>
-      <c r="C136" s="6" t="s">
+      <c r="C136" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D136" s="7">
+      <c r="D136" s="3">
         <v>5</v>
       </c>
       <c r="H136" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="137" spans="1:8" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A137" s="5"/>
-      <c r="B137" s="10">
+    <row r="137" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A137" s="14"/>
+      <c r="B137" s="5">
         <v>136</v>
       </c>
-      <c r="C137" s="11" t="s">
+      <c r="C137" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="D137" s="12">
+      <c r="D137" s="7">
         <v>6</v>
       </c>
-      <c r="E137" s="12"/>
-      <c r="F137" s="10" t="s">
+      <c r="E137" s="7"/>
+      <c r="F137" s="5" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="138" spans="1:8" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A138" s="5"/>
-      <c r="B138" s="10">
+    <row r="138" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A138" s="14"/>
+      <c r="B138" s="5">
         <v>137</v>
       </c>
-      <c r="C138" s="11" t="s">
+      <c r="C138" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="D138" s="12">
+      <c r="D138" s="7">
         <v>7</v>
       </c>
-      <c r="E138" s="12"/>
-      <c r="F138" s="10" t="s">
+      <c r="E138" s="7"/>
+      <c r="F138" s="5" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="139" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A139" s="5"/>
-      <c r="B139" s="13">
+    <row r="139" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A139" s="14"/>
+      <c r="B139" s="8">
         <v>138</v>
       </c>
-      <c r="C139" s="14" t="s">
+      <c r="C139" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="D139" s="15">
+      <c r="D139" s="10">
         <v>0</v>
       </c>
-      <c r="E139" s="15"/>
+      <c r="E139" s="10"/>
     </row>
     <row r="140" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A140" s="5"/>
+      <c r="A140" s="14"/>
       <c r="B140">
         <v>139</v>
       </c>
-      <c r="C140" s="6" t="s">
+      <c r="C140" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D140" s="7">
+      <c r="D140" s="3">
         <v>8</v>
       </c>
       <c r="H140" t="s">
@@ -2895,14 +2898,14 @@
       </c>
     </row>
     <row r="141" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A141" s="5"/>
+      <c r="A141" s="14"/>
       <c r="B141">
         <v>140</v>
       </c>
-      <c r="C141" s="6" t="s">
+      <c r="C141" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D141" s="7">
+      <c r="D141" s="3">
         <v>9</v>
       </c>
       <c r="H141" t="s">
@@ -2910,50 +2913,50 @@
       </c>
     </row>
     <row r="142" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A142" s="5"/>
+      <c r="A142" s="14"/>
       <c r="B142">
         <v>141</v>
       </c>
-      <c r="C142" s="6" t="s">
+      <c r="C142" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D142" s="7">
+      <c r="D142" s="3">
         <v>0</v>
       </c>
     </row>
     <row r="143" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A143" s="5"/>
+      <c r="A143" s="14"/>
       <c r="B143">
         <v>142</v>
       </c>
-      <c r="C143" s="6" t="s">
+      <c r="C143" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D143" s="7">
+      <c r="D143" s="3">
         <v>1</v>
       </c>
     </row>
-    <row r="144" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A144" s="5"/>
-      <c r="B144" s="13">
+    <row r="144" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A144" s="14"/>
+      <c r="B144" s="8">
         <v>143</v>
       </c>
-      <c r="C144" s="14" t="s">
+      <c r="C144" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="D144" s="15"/>
-      <c r="E144" s="15"/>
-    </row>
-    <row r="145" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A145" s="5"/>
-      <c r="B145" s="13">
+      <c r="D144" s="10"/>
+      <c r="E144" s="10"/>
+    </row>
+    <row r="145" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A145" s="14"/>
+      <c r="B145" s="8">
         <v>144</v>
       </c>
-      <c r="C145" s="14" t="s">
+      <c r="C145" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="D145" s="15"/>
-      <c r="E145" s="15"/>
+      <c r="D145" s="10"/>
+      <c r="E145" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -2964,7 +2967,7 @@
     <mergeCell ref="C1:D1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="88" fitToHeight="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2972,15 +2975,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B689E61-58E7-470F-A0EB-580E9AC262B3}">
   <dimension ref="A1:O69"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="L30" sqref="L30"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="1"/>
-    <col min="3" max="3" width="8.42578125" style="6" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.42578125" style="7" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.42578125" style="3" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="1.7109375" customWidth="1"/>
     <col min="6" max="6" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="1.7109375" customWidth="1"/>
@@ -2999,22 +3002,22 @@
       <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="D1" s="9"/>
+      <c r="D1" s="15"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="11" t="s">
         <v>2</v>
       </c>
       <c r="B2">
         <v>1</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="7">
+      <c r="D2" s="3">
         <v>2</v>
       </c>
       <c r="J2" t="s">
@@ -3025,14 +3028,14 @@
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="2"/>
+      <c r="A3" s="11"/>
       <c r="B3">
         <v>2</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="7">
+      <c r="D3" s="3">
         <v>3</v>
       </c>
       <c r="J3" t="s">
@@ -3043,14 +3046,14 @@
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="2"/>
+      <c r="A4" s="11"/>
       <c r="B4">
         <v>3</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="C4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="7">
+      <c r="D4" s="3">
         <v>4</v>
       </c>
       <c r="J4" t="s">
@@ -3061,17 +3064,17 @@
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="2"/>
+      <c r="A5" s="11"/>
       <c r="B5">
         <v>4</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="C5" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="7">
+      <c r="D5" s="3">
         <v>5</v>
       </c>
-      <c r="H5" s="10" t="s">
+      <c r="H5" s="5" t="s">
         <v>79</v>
       </c>
       <c r="J5" t="s">
@@ -3082,17 +3085,17 @@
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="2"/>
+      <c r="A6" s="11"/>
       <c r="B6">
         <v>5</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="C6" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D6" s="7">
+      <c r="D6" s="3">
         <v>6</v>
       </c>
-      <c r="H6" s="10" t="s">
+      <c r="H6" s="5" t="s">
         <v>80</v>
       </c>
       <c r="J6" t="s">
@@ -3103,62 +3106,62 @@
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="2"/>
+      <c r="A7" s="11"/>
       <c r="B7">
         <v>7</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="C7" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="7">
+      <c r="D7" s="3">
         <v>13</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="2"/>
+      <c r="A8" s="11"/>
       <c r="B8">
         <v>10</v>
       </c>
-      <c r="C8" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="D8" s="7">
+      <c r="C8" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D8" s="3">
         <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="2"/>
+      <c r="A9" s="11"/>
       <c r="B9">
         <v>11</v>
       </c>
-      <c r="C9" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="D9" s="7">
+      <c r="C9" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D9" s="3">
         <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="2"/>
+      <c r="A10" s="11"/>
       <c r="B10">
         <v>12</v>
       </c>
-      <c r="C10" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="D10" s="7">
+      <c r="C10" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D10" s="3">
         <v>2</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" s="2"/>
+      <c r="A11" s="11"/>
       <c r="B11">
         <v>13</v>
       </c>
-      <c r="C11" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="D11" s="7">
+      <c r="C11" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D11" s="3">
         <v>3</v>
       </c>
       <c r="F11" t="s">
@@ -3166,14 +3169,14 @@
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="2"/>
+      <c r="A12" s="11"/>
       <c r="B12">
         <v>14</v>
       </c>
-      <c r="C12" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="D12" s="7">
+      <c r="C12" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D12" s="3">
         <v>4</v>
       </c>
       <c r="F12" t="s">
@@ -3181,14 +3184,14 @@
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" s="2"/>
+      <c r="A13" s="11"/>
       <c r="B13">
         <v>15</v>
       </c>
-      <c r="C13" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="D13" s="7">
+      <c r="C13" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D13" s="3">
         <v>5</v>
       </c>
       <c r="F13" t="s">
@@ -3196,14 +3199,14 @@
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14" s="2"/>
+      <c r="A14" s="11"/>
       <c r="B14">
         <v>18</v>
       </c>
-      <c r="C14" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="D14" s="7">
+      <c r="C14" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D14" s="3">
         <v>6</v>
       </c>
       <c r="F14" t="s">
@@ -3211,14 +3214,14 @@
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A15" s="2"/>
+      <c r="A15" s="11"/>
       <c r="B15">
         <v>19</v>
       </c>
-      <c r="C15" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="D15" s="7">
+      <c r="C15" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D15" s="3">
         <v>7</v>
       </c>
       <c r="F15" t="s">
@@ -3226,14 +3229,14 @@
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16" s="2"/>
+      <c r="A16" s="11"/>
       <c r="B16">
         <v>20</v>
       </c>
-      <c r="C16" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="D16" s="7">
+      <c r="C16" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D16" s="3">
         <v>7</v>
       </c>
       <c r="F16" t="s">
@@ -3241,14 +3244,14 @@
       </c>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A17" s="2"/>
+      <c r="A17" s="11"/>
       <c r="B17">
         <v>21</v>
       </c>
-      <c r="C17" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="D17" s="7">
+      <c r="C17" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D17" s="3">
         <v>9</v>
       </c>
       <c r="F17" t="s">
@@ -3256,14 +3259,14 @@
       </c>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A18" s="2"/>
+      <c r="A18" s="11"/>
       <c r="B18">
         <v>22</v>
       </c>
-      <c r="C18" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="D18" s="7">
+      <c r="C18" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D18" s="3">
         <v>10</v>
       </c>
       <c r="F18" t="s">
@@ -3271,14 +3274,14 @@
       </c>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A19" s="2"/>
+      <c r="A19" s="11"/>
       <c r="B19">
         <v>26</v>
       </c>
-      <c r="C19" s="6" t="s">
+      <c r="C19" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D19" s="7">
+      <c r="D19" s="3">
         <v>0</v>
       </c>
       <c r="F19" t="s">
@@ -3286,14 +3289,14 @@
       </c>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A20" s="2"/>
+      <c r="A20" s="11"/>
       <c r="B20">
         <v>27</v>
       </c>
-      <c r="C20" s="6" t="s">
+      <c r="C20" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D20" s="7">
+      <c r="D20" s="3">
         <v>1</v>
       </c>
       <c r="F20" t="s">
@@ -3301,865 +3304,1054 @@
       </c>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A21" s="2"/>
+      <c r="A21" s="11"/>
       <c r="B21">
         <v>28</v>
       </c>
-      <c r="C21" s="6" t="s">
+      <c r="C21" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D21" s="7">
+      <c r="D21" s="3">
         <v>2</v>
       </c>
-      <c r="H21" s="10" t="s">
+      <c r="F21" s="5"/>
+      <c r="G21" s="5"/>
+      <c r="H21" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="J21" t="s">
+      <c r="I21" s="5"/>
+      <c r="J21" s="5" t="s">
         <v>132</v>
       </c>
-      <c r="K21" t="s">
+      <c r="K21" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="L21" t="s">
+      <c r="L21" s="5" t="s">
         <v>135</v>
       </c>
-      <c r="N21" t="s">
+      <c r="M21" s="5"/>
+      <c r="N21" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="O21">
+      <c r="O21" s="5">
         <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A22" s="2"/>
+      <c r="A22" s="11"/>
       <c r="B22">
         <v>29</v>
       </c>
-      <c r="C22" s="6" t="s">
+      <c r="C22" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D22" s="7">
+      <c r="D22" s="3">
         <v>3</v>
       </c>
-      <c r="H22" s="10" t="s">
+      <c r="F22" s="5"/>
+      <c r="G22" s="5"/>
+      <c r="H22" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="J22" t="s">
+      <c r="I22" s="5"/>
+      <c r="J22" s="5" t="s">
         <v>132</v>
       </c>
-      <c r="K22" t="s">
+      <c r="K22" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="L22" t="s">
+      <c r="L22" s="5" t="s">
         <v>135</v>
       </c>
-      <c r="N22" t="s">
+      <c r="M22" s="5"/>
+      <c r="N22" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="O22">
+      <c r="O22" s="5">
         <v>2</v>
       </c>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A23" s="2"/>
+      <c r="A23" s="11"/>
       <c r="B23">
         <v>36</v>
       </c>
-      <c r="C23" s="6" t="s">
+      <c r="C23" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D23" s="7">
+      <c r="D23" s="3">
         <v>2</v>
       </c>
-      <c r="H23" s="10" t="s">
+      <c r="F23" s="5"/>
+      <c r="G23" s="5"/>
+      <c r="H23" s="5" t="s">
         <v>113</v>
       </c>
-      <c r="J23" t="s">
+      <c r="I23" s="5"/>
+      <c r="J23" s="5" t="s">
         <v>132</v>
       </c>
-      <c r="K23" t="s">
+      <c r="K23" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="L23" t="s">
+      <c r="L23" s="5" t="s">
         <v>133</v>
       </c>
-      <c r="N23" t="s">
+      <c r="M23" s="5"/>
+      <c r="N23" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="O23">
+      <c r="O23" s="5">
         <v>3</v>
       </c>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A24" s="3" t="s">
+      <c r="A24" s="12" t="s">
         <v>3</v>
       </c>
       <c r="B24">
         <v>37</v>
       </c>
-      <c r="C24" s="6" t="s">
+      <c r="C24" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D24" s="7">
+      <c r="D24" s="3">
         <v>3</v>
       </c>
-      <c r="H24" s="10" t="s">
+      <c r="F24" s="5"/>
+      <c r="G24" s="5"/>
+      <c r="H24" s="5" t="s">
         <v>114</v>
       </c>
-      <c r="J24" t="s">
+      <c r="I24" s="5"/>
+      <c r="J24" s="5" t="s">
         <v>132</v>
       </c>
-      <c r="K24" t="s">
+      <c r="K24" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="L24" t="s">
+      <c r="L24" s="5" t="s">
         <v>133</v>
       </c>
-      <c r="N24" t="s">
+      <c r="M24" s="5"/>
+      <c r="N24" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="O24">
+      <c r="O24" s="5">
         <v>4</v>
       </c>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A25" s="3"/>
+      <c r="A25" s="12"/>
       <c r="B25">
         <v>40</v>
       </c>
-      <c r="C25" s="6" t="s">
+      <c r="C25" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D25" s="7">
+      <c r="D25" s="3">
         <v>4</v>
       </c>
-      <c r="F25" t="s">
+      <c r="F25" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="H25" s="10" t="s">
+      <c r="G25" s="5"/>
+      <c r="H25" s="5" t="s">
         <v>138</v>
       </c>
-      <c r="J25" t="s">
+      <c r="I25" s="5"/>
+      <c r="J25" s="5" t="s">
         <v>136</v>
       </c>
-      <c r="K25" t="s">
+      <c r="K25" s="5" t="s">
         <v>137</v>
       </c>
+      <c r="L25" s="5"/>
+      <c r="M25" s="5"/>
+      <c r="N25" s="5"/>
+      <c r="O25" s="5"/>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A26" s="3"/>
+      <c r="A26" s="12"/>
       <c r="B26">
         <v>44</v>
       </c>
-      <c r="C26" s="6" t="s">
+      <c r="C26" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D26" s="7">
+      <c r="D26" s="3">
         <v>4</v>
       </c>
-      <c r="H26" s="10" t="s">
+      <c r="F26" s="5"/>
+      <c r="G26" s="5"/>
+      <c r="H26" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="J26" t="s">
+      <c r="I26" s="5"/>
+      <c r="J26" s="5" t="s">
         <v>132</v>
       </c>
-      <c r="K26" t="s">
+      <c r="K26" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="L26" t="s">
+      <c r="L26" s="5" t="s">
         <v>135</v>
       </c>
-      <c r="N26" t="s">
+      <c r="M26" s="5"/>
+      <c r="N26" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="O26">
+      <c r="O26" s="5">
         <v>1</v>
       </c>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A27" s="3"/>
+      <c r="A27" s="12"/>
       <c r="B27">
         <v>45</v>
       </c>
-      <c r="C27" s="6" t="s">
+      <c r="C27" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D27" s="7">
+      <c r="D27" s="3">
         <v>5</v>
       </c>
-      <c r="H27" s="10" t="s">
+      <c r="F27" s="5"/>
+      <c r="G27" s="5"/>
+      <c r="H27" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="J27" t="s">
+      <c r="I27" s="5"/>
+      <c r="J27" s="5" t="s">
         <v>132</v>
       </c>
-      <c r="K27" t="s">
+      <c r="K27" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="L27" t="s">
+      <c r="L27" s="5" t="s">
         <v>135</v>
       </c>
-      <c r="N27" t="s">
+      <c r="M27" s="5"/>
+      <c r="N27" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="O27">
+      <c r="O27" s="5">
         <v>2</v>
       </c>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A28" s="3"/>
+      <c r="A28" s="12"/>
       <c r="B28">
         <v>49</v>
       </c>
-      <c r="C28" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="D28" s="7">
+      <c r="C28" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D28" s="3">
         <v>11</v>
       </c>
-      <c r="N28" t="s">
+      <c r="F28" s="5"/>
+      <c r="G28" s="5"/>
+      <c r="H28" s="5"/>
+      <c r="I28" s="5"/>
+      <c r="J28" s="5"/>
+      <c r="K28" s="5"/>
+      <c r="L28" s="5"/>
+      <c r="M28" s="5"/>
+      <c r="N28" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="O28">
+      <c r="O28" s="5">
         <v>5</v>
       </c>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A29" s="3"/>
+      <c r="A29" s="12"/>
       <c r="B29">
         <v>50</v>
       </c>
-      <c r="C29" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="D29" s="7">
+      <c r="C29" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D29" s="3">
         <v>12</v>
       </c>
-      <c r="N29" t="s">
+      <c r="F29" s="5"/>
+      <c r="G29" s="5"/>
+      <c r="H29" s="5"/>
+      <c r="I29" s="5"/>
+      <c r="J29" s="5"/>
+      <c r="K29" s="5"/>
+      <c r="L29" s="5"/>
+      <c r="M29" s="5"/>
+      <c r="N29" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="O29">
+      <c r="O29" s="5">
         <v>6</v>
       </c>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A30" s="3"/>
+      <c r="A30" s="12"/>
       <c r="B30">
         <v>53</v>
       </c>
-      <c r="C30" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="D30" s="7">
+      <c r="C30" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D30" s="3">
         <v>13</v>
       </c>
-      <c r="N30" t="s">
+      <c r="F30" s="5"/>
+      <c r="G30" s="5"/>
+      <c r="H30" s="5"/>
+      <c r="I30" s="5"/>
+      <c r="J30" s="5"/>
+      <c r="K30" s="5"/>
+      <c r="L30" s="5"/>
+      <c r="M30" s="5"/>
+      <c r="N30" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="O30">
+      <c r="O30" s="5">
         <v>7</v>
       </c>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A31" s="3"/>
+      <c r="A31" s="12"/>
       <c r="B31">
         <v>54</v>
       </c>
-      <c r="C31" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="D31" s="7">
+      <c r="C31" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D31" s="3">
         <v>14</v>
       </c>
-      <c r="N31" t="s">
+      <c r="F31" s="5"/>
+      <c r="G31" s="5"/>
+      <c r="H31" s="5"/>
+      <c r="I31" s="5"/>
+      <c r="J31" s="5"/>
+      <c r="K31" s="5"/>
+      <c r="L31" s="5"/>
+      <c r="M31" s="5"/>
+      <c r="N31" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="O31">
+      <c r="O31" s="5">
         <v>8</v>
       </c>
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A32" s="3"/>
+      <c r="A32" s="12"/>
       <c r="B32">
         <v>55</v>
       </c>
-      <c r="C32" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="D32" s="7">
+      <c r="C32" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D32" s="3">
         <v>15</v>
       </c>
-      <c r="N32" t="s">
+      <c r="F32" s="5"/>
+      <c r="G32" s="5"/>
+      <c r="H32" s="5"/>
+      <c r="I32" s="5"/>
+      <c r="J32" s="5"/>
+      <c r="K32" s="5"/>
+      <c r="L32" s="5"/>
+      <c r="M32" s="5"/>
+      <c r="N32" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="O32">
+      <c r="O32" s="5">
         <v>9</v>
       </c>
     </row>
     <row r="33" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A33" s="3"/>
+      <c r="A33" s="12"/>
       <c r="B33">
         <v>56</v>
       </c>
-      <c r="C33" s="6" t="s">
+      <c r="C33" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D33" s="7">
+      <c r="D33" s="3">
         <v>0</v>
       </c>
-      <c r="N33" t="s">
+      <c r="F33" s="5"/>
+      <c r="G33" s="5"/>
+      <c r="H33" s="5"/>
+      <c r="I33" s="5"/>
+      <c r="J33" s="5"/>
+      <c r="K33" s="5"/>
+      <c r="L33" s="5"/>
+      <c r="M33" s="5"/>
+      <c r="N33" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="O33">
+      <c r="O33" s="5">
         <v>10</v>
       </c>
     </row>
     <row r="34" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A34" s="3"/>
+      <c r="A34" s="12"/>
       <c r="B34">
         <v>57</v>
       </c>
-      <c r="C34" s="6" t="s">
+      <c r="C34" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D34" s="7">
+      <c r="D34" s="3">
         <v>1</v>
       </c>
-      <c r="N34" t="s">
+      <c r="F34" s="5"/>
+      <c r="G34" s="5"/>
+      <c r="H34" s="5"/>
+      <c r="I34" s="5"/>
+      <c r="J34" s="5"/>
+      <c r="K34" s="5"/>
+      <c r="L34" s="5"/>
+      <c r="M34" s="5"/>
+      <c r="N34" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="O34" t="s">
+      <c r="O34" s="5" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="35" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A35" s="3"/>
+      <c r="A35" s="12"/>
       <c r="B35">
         <v>60</v>
       </c>
-      <c r="C35" s="6" t="s">
+      <c r="C35" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D35" s="7">
-        <v>9</v>
-      </c>
-      <c r="N35" t="s">
+      <c r="D35" s="3">
+        <v>9</v>
+      </c>
+      <c r="F35" s="5"/>
+      <c r="G35" s="5"/>
+      <c r="H35" s="5"/>
+      <c r="I35" s="5"/>
+      <c r="J35" s="5"/>
+      <c r="K35" s="5"/>
+      <c r="L35" s="5"/>
+      <c r="M35" s="5"/>
+      <c r="N35" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="O35" t="s">
+      <c r="O35" s="5" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="36" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A36" s="3"/>
+      <c r="A36" s="12"/>
       <c r="B36">
         <v>63</v>
       </c>
-      <c r="C36" s="6" t="s">
+      <c r="C36" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D36" s="7">
+      <c r="D36" s="3">
         <v>10</v>
       </c>
-      <c r="N36" t="s">
+      <c r="F36" s="5"/>
+      <c r="G36" s="5"/>
+      <c r="H36" s="5"/>
+      <c r="I36" s="5"/>
+      <c r="J36" s="5"/>
+      <c r="K36" s="5"/>
+      <c r="L36" s="5"/>
+      <c r="M36" s="5"/>
+      <c r="N36" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="O36" t="s">
+      <c r="O36" s="5" t="s">
         <v>143</v>
       </c>
     </row>
     <row r="37" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A37" s="3"/>
+      <c r="A37" s="12"/>
       <c r="B37">
         <v>64</v>
       </c>
-      <c r="C37" s="6" t="s">
+      <c r="C37" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D37" s="7">
+      <c r="D37" s="3">
         <v>11</v>
       </c>
-      <c r="H37" s="10" t="s">
+      <c r="F37" s="5"/>
+      <c r="G37" s="5"/>
+      <c r="H37" s="5" t="s">
         <v>139</v>
       </c>
-      <c r="J37" t="s">
+      <c r="I37" s="5"/>
+      <c r="J37" s="5" t="s">
         <v>140</v>
       </c>
-      <c r="K37" t="s">
+      <c r="K37" s="5" t="s">
         <v>137</v>
       </c>
+      <c r="L37" s="5"/>
+      <c r="M37" s="5"/>
+      <c r="N37" s="5"/>
+      <c r="O37" s="5"/>
     </row>
     <row r="38" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A38" s="3"/>
+      <c r="A38" s="12"/>
       <c r="B38">
         <v>68</v>
       </c>
-      <c r="C38" s="6" t="s">
+      <c r="C38" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D38" s="7">
+      <c r="D38" s="3">
         <v>15</v>
       </c>
-      <c r="N38" t="s">
+      <c r="F38" s="5"/>
+      <c r="G38" s="5"/>
+      <c r="H38" s="5"/>
+      <c r="I38" s="5"/>
+      <c r="J38" s="5"/>
+      <c r="K38" s="5"/>
+      <c r="L38" s="5"/>
+      <c r="M38" s="5"/>
+      <c r="N38" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="O38">
+      <c r="O38" s="5">
         <v>5</v>
       </c>
     </row>
     <row r="39" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A39" s="4"/>
+      <c r="A39" s="13"/>
       <c r="B39">
         <v>76</v>
       </c>
-      <c r="C39" s="6" t="s">
+      <c r="C39" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D39" s="7">
+      <c r="D39" s="3">
         <v>15</v>
       </c>
-      <c r="N39" t="s">
+      <c r="F39" s="5"/>
+      <c r="G39" s="5"/>
+      <c r="H39" s="5"/>
+      <c r="I39" s="5"/>
+      <c r="J39" s="5"/>
+      <c r="K39" s="5"/>
+      <c r="L39" s="5"/>
+      <c r="M39" s="5"/>
+      <c r="N39" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="O39">
+      <c r="O39" s="5">
         <v>6</v>
       </c>
     </row>
     <row r="40" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A40" s="4"/>
+      <c r="A40" s="13"/>
       <c r="B40">
         <v>79</v>
       </c>
-      <c r="C40" s="6" t="s">
+      <c r="C40" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="D40" s="7">
+      <c r="D40" s="3">
         <v>10</v>
       </c>
-      <c r="N40" t="s">
+      <c r="F40" s="5"/>
+      <c r="G40" s="5"/>
+      <c r="H40" s="5"/>
+      <c r="I40" s="5"/>
+      <c r="J40" s="5"/>
+      <c r="K40" s="5"/>
+      <c r="L40" s="5"/>
+      <c r="M40" s="5"/>
+      <c r="N40" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="O40">
+      <c r="O40" s="5">
         <v>7</v>
       </c>
     </row>
     <row r="41" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A41" s="4"/>
+      <c r="A41" s="13"/>
       <c r="B41">
         <v>81</v>
       </c>
-      <c r="C41" s="6" t="s">
+      <c r="C41" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="D41" s="7">
+      <c r="D41" s="3">
         <v>12</v>
       </c>
-      <c r="H41" s="10" t="s">
+      <c r="F41" s="5"/>
+      <c r="G41" s="5"/>
+      <c r="H41" s="5" t="s">
         <v>103</v>
       </c>
-      <c r="J41" t="s">
+      <c r="I41" s="5"/>
+      <c r="J41" s="5" t="s">
         <v>132</v>
       </c>
-      <c r="K41" t="s">
+      <c r="K41" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="L41" t="s">
+      <c r="L41" s="5" t="s">
         <v>133</v>
       </c>
-      <c r="N41" t="s">
+      <c r="M41" s="5"/>
+      <c r="N41" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="O41">
+      <c r="O41" s="5">
         <v>3</v>
       </c>
     </row>
     <row r="42" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A42" s="4"/>
+      <c r="A42" s="13"/>
       <c r="B42">
         <v>82</v>
       </c>
-      <c r="C42" s="6" t="s">
+      <c r="C42" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="D42" s="7">
+      <c r="D42" s="3">
         <v>13</v>
       </c>
-      <c r="H42" s="10" t="s">
+      <c r="F42" s="5"/>
+      <c r="G42" s="5"/>
+      <c r="H42" s="5" t="s">
         <v>104</v>
       </c>
-      <c r="J42" t="s">
+      <c r="I42" s="5"/>
+      <c r="J42" s="5" t="s">
         <v>132</v>
       </c>
-      <c r="K42" t="s">
+      <c r="K42" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="L42" t="s">
+      <c r="L42" s="5" t="s">
         <v>133</v>
       </c>
-      <c r="N42" t="s">
+      <c r="M42" s="5"/>
+      <c r="N42" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="O42">
+      <c r="O42" s="5">
         <v>4</v>
       </c>
     </row>
     <row r="43" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A43" s="4"/>
+      <c r="A43" s="13"/>
       <c r="B43">
         <v>85</v>
       </c>
-      <c r="C43" s="6" t="s">
+      <c r="C43" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="D43" s="7">
+      <c r="D43" s="3">
         <v>14</v>
       </c>
-      <c r="N43" t="s">
+      <c r="F43" s="5"/>
+      <c r="G43" s="5"/>
+      <c r="H43" s="5"/>
+      <c r="I43" s="5"/>
+      <c r="J43" s="5"/>
+      <c r="K43" s="5"/>
+      <c r="L43" s="5"/>
+      <c r="M43" s="5"/>
+      <c r="N43" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="O43">
+      <c r="O43" s="5">
         <v>8</v>
       </c>
     </row>
     <row r="44" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A44" s="4"/>
+      <c r="A44" s="13"/>
       <c r="B44">
         <v>86</v>
       </c>
-      <c r="C44" s="6" t="s">
+      <c r="C44" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="D44" s="7">
+      <c r="D44" s="3">
         <v>15</v>
       </c>
-      <c r="N44" t="s">
+      <c r="F44" s="5"/>
+      <c r="G44" s="5"/>
+      <c r="H44" s="5"/>
+      <c r="I44" s="5"/>
+      <c r="J44" s="5"/>
+      <c r="K44" s="5"/>
+      <c r="L44" s="5"/>
+      <c r="M44" s="5"/>
+      <c r="N44" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="O44">
+      <c r="O44" s="5">
         <v>9</v>
       </c>
     </row>
     <row r="45" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A45" s="4"/>
+      <c r="A45" s="13"/>
       <c r="B45">
         <v>87</v>
       </c>
-      <c r="C45" s="6" t="s">
+      <c r="C45" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D45" s="7">
+      <c r="D45" s="3">
         <v>2</v>
       </c>
-      <c r="N45" t="s">
+      <c r="F45" s="5"/>
+      <c r="G45" s="5"/>
+      <c r="H45" s="5"/>
+      <c r="I45" s="5"/>
+      <c r="J45" s="5"/>
+      <c r="K45" s="5"/>
+      <c r="L45" s="5"/>
+      <c r="M45" s="5"/>
+      <c r="N45" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="O45">
+      <c r="O45" s="5">
         <v>10</v>
       </c>
     </row>
     <row r="46" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A46" s="4"/>
+      <c r="A46" s="13"/>
       <c r="B46">
         <v>88</v>
       </c>
-      <c r="C46" s="6" t="s">
+      <c r="C46" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D46" s="7">
+      <c r="D46" s="3">
         <v>3</v>
       </c>
-      <c r="N46" t="s">
+      <c r="F46" s="5"/>
+      <c r="G46" s="5"/>
+      <c r="H46" s="5"/>
+      <c r="I46" s="5"/>
+      <c r="J46" s="5"/>
+      <c r="K46" s="5"/>
+      <c r="L46" s="5"/>
+      <c r="M46" s="5"/>
+      <c r="N46" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="O46" t="s">
+      <c r="O46" s="5" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="47" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A47" s="4"/>
+      <c r="A47" s="13"/>
       <c r="B47">
         <v>89</v>
       </c>
-      <c r="C47" s="6" t="s">
+      <c r="C47" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D47" s="7">
+      <c r="D47" s="3">
         <v>4</v>
       </c>
-      <c r="N47" t="s">
+      <c r="F47" s="5"/>
+      <c r="G47" s="5"/>
+      <c r="H47" s="5"/>
+      <c r="I47" s="5"/>
+      <c r="J47" s="5"/>
+      <c r="K47" s="5"/>
+      <c r="L47" s="5"/>
+      <c r="M47" s="5"/>
+      <c r="N47" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="O47" t="s">
+      <c r="O47" s="5" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="48" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A48" s="4"/>
+      <c r="A48" s="13"/>
       <c r="B48">
         <v>90</v>
       </c>
-      <c r="C48" s="6" t="s">
+      <c r="C48" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D48" s="7">
+      <c r="D48" s="3">
         <v>5</v>
       </c>
-      <c r="N48" t="s">
+      <c r="F48" s="5"/>
+      <c r="G48" s="5"/>
+      <c r="H48" s="5"/>
+      <c r="I48" s="5"/>
+      <c r="J48" s="5"/>
+      <c r="K48" s="5"/>
+      <c r="L48" s="5"/>
+      <c r="M48" s="5"/>
+      <c r="N48" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="O48" t="s">
+      <c r="O48" s="5" t="s">
         <v>143</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A49" s="4"/>
+      <c r="A49" s="13"/>
       <c r="B49">
         <v>91</v>
       </c>
-      <c r="C49" s="6" t="s">
+      <c r="C49" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D49" s="7">
+      <c r="D49" s="3">
         <v>6</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A50" s="4"/>
+      <c r="A50" s="13"/>
       <c r="B50">
         <v>92</v>
       </c>
-      <c r="C50" s="6" t="s">
+      <c r="C50" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D50" s="7">
+      <c r="D50" s="3">
         <v>7</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A51" s="4"/>
+      <c r="A51" s="13"/>
       <c r="B51">
         <v>93</v>
       </c>
-      <c r="C51" s="6" t="s">
+      <c r="C51" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D51" s="7">
+      <c r="D51" s="3">
         <v>8</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A52" s="4"/>
+      <c r="A52" s="13"/>
       <c r="B52">
         <v>96</v>
       </c>
-      <c r="C52" s="6" t="s">
+      <c r="C52" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D52" s="7">
+      <c r="D52" s="3">
         <v>6</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A53" s="4"/>
+      <c r="A53" s="13"/>
       <c r="B53">
         <v>97</v>
       </c>
-      <c r="C53" s="6" t="s">
+      <c r="C53" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D53" s="7">
+      <c r="D53" s="3">
         <v>7</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A54" s="5"/>
+      <c r="A54" s="14"/>
       <c r="B54">
         <v>111</v>
       </c>
-      <c r="C54" s="6" t="s">
+      <c r="C54" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D54" s="7">
+      <c r="D54" s="3">
         <v>10</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A55" s="5"/>
+      <c r="A55" s="14"/>
       <c r="B55">
         <v>113</v>
       </c>
-      <c r="C55" s="6" t="s">
+      <c r="C55" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D55" s="7">
+      <c r="D55" s="3">
         <v>12</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A56" s="5"/>
+      <c r="A56" s="14"/>
       <c r="B56">
         <v>123</v>
       </c>
-      <c r="C56" s="6" t="s">
+      <c r="C56" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="D56" s="7">
+      <c r="D56" s="3">
         <v>7</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A57" s="5"/>
+      <c r="A57" s="14"/>
       <c r="B57">
         <v>124</v>
       </c>
-      <c r="C57" s="6" t="s">
+      <c r="C57" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D57" s="7">
+      <c r="D57" s="3">
         <v>9</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A58" s="5"/>
+      <c r="A58" s="14"/>
       <c r="B58">
         <v>125</v>
       </c>
-      <c r="C58" s="6" t="s">
+      <c r="C58" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D58" s="7">
+      <c r="D58" s="3">
         <v>10</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A59" s="5"/>
+      <c r="A59" s="14"/>
       <c r="B59">
         <v>126</v>
       </c>
-      <c r="C59" s="6" t="s">
+      <c r="C59" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D59" s="7">
+      <c r="D59" s="3">
         <v>11</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A60" s="5"/>
+      <c r="A60" s="14"/>
       <c r="B60">
         <v>127</v>
       </c>
-      <c r="C60" s="6" t="s">
+      <c r="C60" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D60" s="7">
+      <c r="D60" s="3">
         <v>12</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A61" s="5"/>
+      <c r="A61" s="14"/>
       <c r="B61">
         <v>128</v>
       </c>
-      <c r="C61" s="6" t="s">
+      <c r="C61" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D61" s="7">
+      <c r="D61" s="3">
         <v>13</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A62" s="5"/>
+      <c r="A62" s="14"/>
       <c r="B62">
         <v>129</v>
       </c>
-      <c r="C62" s="6" t="s">
+      <c r="C62" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D62" s="7">
+      <c r="D62" s="3">
         <v>14</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A63" s="5"/>
+      <c r="A63" s="14"/>
       <c r="B63">
         <v>132</v>
       </c>
-      <c r="C63" s="6" t="s">
+      <c r="C63" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D63" s="7">
+      <c r="D63" s="3">
         <v>15</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A64" s="5"/>
+      <c r="A64" s="14"/>
       <c r="B64">
         <v>134</v>
       </c>
-      <c r="C64" s="6" t="s">
+      <c r="C64" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D64" s="7">
+      <c r="D64" s="3">
         <v>4</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A65" s="5"/>
+      <c r="A65" s="14"/>
       <c r="B65">
         <v>135</v>
       </c>
-      <c r="C65" s="6" t="s">
+      <c r="C65" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D65" s="7">
+      <c r="D65" s="3">
         <v>5</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A66" s="5"/>
+      <c r="A66" s="14"/>
       <c r="B66">
         <v>139</v>
       </c>
-      <c r="C66" s="6" t="s">
+      <c r="C66" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D66" s="7">
+      <c r="D66" s="3">
         <v>8</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A67" s="5"/>
+      <c r="A67" s="14"/>
       <c r="B67">
         <v>140</v>
       </c>
-      <c r="C67" s="6" t="s">
+      <c r="C67" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D67" s="7">
+      <c r="D67" s="3">
         <v>9</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A68" s="5"/>
+      <c r="A68" s="14"/>
       <c r="B68">
         <v>141</v>
       </c>
-      <c r="C68" s="6" t="s">
+      <c r="C68" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D68" s="7">
+      <c r="D68" s="3">
         <v>0</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A69" s="5"/>
+      <c r="A69" s="14"/>
       <c r="B69">
         <v>142</v>
       </c>
-      <c r="C69" s="6" t="s">
+      <c r="C69" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D69" s="7">
+      <c r="D69" s="3">
         <v>1</v>
       </c>
     </row>

</xml_diff>